<commit_message>
corrected to excel feature
</commit_message>
<xml_diff>
--- a/file_transformation_service/out/generated_data_frame.xlsx
+++ b/file_transformation_service/out/generated_data_frame.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,32 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>data</t>
+          <t>firstname</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>lastname</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>address1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>address2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>address4</t>
         </is>
       </c>
     </row>
@@ -446,7 +471,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'firstname': 'John', 'lastname': 'Doe', 'address1': '120 jefferson st.', 'address2': 'Riverside', 'address3': ' NJ', 'address4': ' 08075'}</t>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>120 jefferson st.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> NJ</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 08075</t>
         </is>
       </c>
     </row>
@@ -456,7 +506,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{'firstname': 'Jack', 'lastname': 'McGinnis', 'address1': '220 hobo Av.', 'address2': 'Phila', 'address3': ' PA', 'address4': '09119'}</t>
+          <t>Jack</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>McGinnis</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>220 hobo Av.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Phila</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PA</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>09119</t>
         </is>
       </c>
     </row>
@@ -466,7 +541,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{'firstname': 'John "Da Man"', 'lastname': 'Repici', 'address1': '120 Jefferson St.', 'address2': 'Riverside', 'address3': ' NJ', 'address4': '08075'}</t>
+          <t>John "Da Man"</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Repici</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>120 Jefferson St.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Riverside</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> NJ</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>08075</t>
         </is>
       </c>
     </row>
@@ -476,7 +576,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{'firstname': 'Stephen', 'lastname': 'Tyler', 'address1': '7452 Terrace "At the Plaza" road', 'address2': 'SomeTown', 'address3': 'SD', 'address4': ' 91234'}</t>
+          <t>Stephen</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Tyler</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>7452 Terrace "At the Plaza" road</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SomeTown</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 91234</t>
         </is>
       </c>
     </row>
@@ -484,9 +609,26 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>{'firstname': '', 'lastname': 'Blankman', 'address1': '', 'address2': 'SomeTown', 'address3': ' SD', 'address4': ' 00298'}</t>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Blankman</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SomeTown</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SD</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 00298</t>
         </is>
       </c>
     </row>
@@ -496,7 +638,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'firstname': 'Joan "the bone", Anne', 'lastname': 'Jet', 'address1': '9th, at Terrace plc', 'address2': 'Desert City', 'address3': 'CO', 'address4': '00123'}</t>
+          <t>Joan "the bone", Anne</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Jet</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>9th, at Terrace plc</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Desert City</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>00123</t>
         </is>
       </c>
     </row>

</xml_diff>